<commit_message>
Updated with platform information.
</commit_message>
<xml_diff>
--- a/source/quickstart/SampleTestbedFile.xlsx
+++ b/source/quickstart/SampleTestbedFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kacann\Documents\development\pyats\userguide\source\quickstart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE7ACF3A-47CC-4FEF-80F0-1C1E41ABE637}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE79F086-2C6D-4D80-A293-CDE4704CB46B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22065" windowHeight="8430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2240" yWindow="2240" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>ip</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>enable_password</t>
+  </si>
+  <si>
+    <t>platform</t>
   </si>
 </sst>
 </file>
@@ -363,23 +366,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="14.26953125" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11.81640625" customWidth="1"/>
+    <col min="4" max="4" width="12.26953125" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" customWidth="1"/>
+    <col min="7" max="7" width="17.26953125" customWidth="1"/>
+    <col min="8" max="8" width="21.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -400,6 +404,9 @@
       </c>
       <c r="G1" t="s">
         <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>